<commit_message>
ready for the report
</commit_message>
<xml_diff>
--- a/Project4/andrewsAlgo/competition results.xlsx
+++ b/Project4/andrewsAlgo/competition results.xlsx
@@ -77,7 +77,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,12 +85,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,7 +390,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,90 +401,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>4949</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>6974</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>0.13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>11455</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>1.95</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>15137</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>14.26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>28685</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>0.40500000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>40933</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>1.53</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>63780</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>9.3000000000000007</v>
       </c>
     </row>

</xml_diff>